<commit_message>
[feature] agregar columnas a la tabla de solicitudes de linea de credito y modificacion de anexo de linea de creditos
</commit_message>
<xml_diff>
--- a/src/assets/anexos/Anexo_Lineas_de_Credito_IFIS.xlsx
+++ b/src/assets/anexos/Anexo_Lineas_de_Credito_IFIS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/papamacone/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/papamacone/Documents/Edgar/coop-ifi-front-center/src/assets/anexos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0354E4A2-8F7A-3341-8D10-56948A485D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6ED3DB-598A-6F4D-A685-D8858C92B1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10300" xr2:uid="{34CE6F97-8127-4792-84FB-86D281043B72}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="19320" xr2:uid="{34CE6F97-8127-4792-84FB-86D281043B72}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -164,7 +164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -175,6 +175,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -493,25 +499,26 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="4"/>
     <col min="6" max="6" width="15.1640625" customWidth="1"/>
     <col min="7" max="7" width="14.83203125" customWidth="1"/>
     <col min="8" max="8" width="15.1640625" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="4" customWidth="1"/>
     <col min="10" max="10" width="15.33203125" customWidth="1"/>
     <col min="11" max="11" width="14.6640625" customWidth="1"/>
-    <col min="12" max="12" width="15.5" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5" style="4" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -523,7 +530,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -535,7 +542,7 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -544,10 +551,10 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">

</xml_diff>